<commit_message>
cleaning up pipeline; sampling complete; running new models
</commit_message>
<xml_diff>
--- a/experiments/dependency_format/dependency_format_experiment-all_ns-spearman.xlsx
+++ b/experiments/dependency_format/dependency_format_experiment-all_ns-spearman.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leviking/Documents/dissertation/SAILS/experiments/dependency_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7BE5A76-336F-CE42-9327-03FE646ED43A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7886703E-9B52-374D-9D74-A9265B2398C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="1460" windowWidth="19440" windowHeight="10840"/>
+    <workbookView xWindow="2720" yWindow="2580" windowWidth="22880" windowHeight="12680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dependency_format_experiment-al" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -232,7 +240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1096,14 +1104,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2517,7 +2530,7 @@
         <v>0.47778896267021609</v>
       </c>
       <c r="C62" s="3">
-        <f t="shared" ref="C62:M62" si="0">(SUM(C2:C61)/60)</f>
+        <f t="shared" ref="C62:G62" si="0">(SUM(C2:C61)/60)</f>
         <v>3.9135651107673315E-2</v>
       </c>
       <c r="D62" s="4">
@@ -2546,7 +2559,7 @@
         <v>0.48042905580599998</v>
       </c>
       <c r="C63" s="3">
-        <f t="shared" ref="C63:M63" si="1">(SUMPRODUCT(ABS(C2:C61))/60)</f>
+        <f t="shared" ref="C63:G63" si="1">(SUMPRODUCT(ABS(C2:C61))/60)</f>
         <v>3.9135651107673315E-2</v>
       </c>
       <c r="D63" s="3">

</xml_diff>